<commit_message>
moved sediment vol to Cburial repo so this is bathym
</commit_message>
<xml_diff>
--- a/Output_Files/Sediment_Volume/pond_area_27dec2023.xlsx
+++ b/Output_Files/Sediment_Volume/pond_area_27dec2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/altagannon/OneDrive/Holgerson_Lab/DEC_Ponds/Output_Files/Sediment_Volume/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3788F21-640E-9A47-8F10-54A750C5715A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7CB06E-F982-7245-8E6D-0B620C4E708A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="26480" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Pond_Name</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Pond_Area_hectares</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -699,9 +702,8 @@
       <c r="B17">
         <v>1364.7806768720038</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0.13647806768720039</v>
+      <c r="C17" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>